<commit_message>
chor: added new pnls
</commit_message>
<xml_diff>
--- a/public/assets/P&L_Report_AF324232333_2182_EQ.xlsx
+++ b/public/assets/P&L_Report_AF324232333_2182_EQ.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/code/tradingpnl/public/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84288A22-4D53-B84E-80F6-264AAD107132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB4B43EA-E57B-5645-8629-78090BA43BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34680" windowHeight="19920" tabRatio="212" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="16380" windowHeight="8200" tabRatio="212" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P&amp;L Details" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="215">
   <si>
     <t>RKSV SECURITIES INDIA PVT LTD</t>
   </si>
@@ -247,6 +248,21 @@
     <t>29-04-2021</t>
   </si>
   <si>
+    <t>CENTRAL DEPO SER (I) LTD</t>
+  </si>
+  <si>
+    <t>CDSL</t>
+  </si>
+  <si>
+    <t>INE736A01011</t>
+  </si>
+  <si>
+    <t>30-04-2021</t>
+  </si>
+  <si>
+    <t>05-10-2021</t>
+  </si>
+  <si>
     <t>CHAMBAL FERTILISERS AND CHEMIC</t>
   </si>
   <si>
@@ -256,6 +272,15 @@
     <t>INE085A01013</t>
   </si>
   <si>
+    <t>DAAWAT</t>
+  </si>
+  <si>
+    <t>INE818H01012</t>
+  </si>
+  <si>
+    <t>17-09-2021</t>
+  </si>
+  <si>
     <t>DELTA CORP</t>
   </si>
   <si>
@@ -289,6 +314,30 @@
     <t>13-08-2021</t>
   </si>
   <si>
+    <t>07-09-2021</t>
+  </si>
+  <si>
+    <t>27-08-2021</t>
+  </si>
+  <si>
+    <t>FILATE INDIA(BSE INDONEXT)</t>
+  </si>
+  <si>
+    <t>FILATEX</t>
+  </si>
+  <si>
+    <t>INE816B01019</t>
+  </si>
+  <si>
+    <t>09-09-2021</t>
+  </si>
+  <si>
+    <t>15-09-2021</t>
+  </si>
+  <si>
+    <t>INE816B01027</t>
+  </si>
+  <si>
     <t>FINOLEX IND</t>
   </si>
   <si>
@@ -418,6 +467,18 @@
     <t>INE389H01014</t>
   </si>
   <si>
+    <t>KNR CONST</t>
+  </si>
+  <si>
+    <t>KNRCON</t>
+  </si>
+  <si>
+    <t>INE634I01011</t>
+  </si>
+  <si>
+    <t>INE634I01029</t>
+  </si>
+  <si>
     <t>LAURUSLABS</t>
   </si>
   <si>
@@ -484,6 +545,24 @@
     <t>INE195J01029</t>
   </si>
   <si>
+    <t>POWER MECH PROJECTS LTD.</t>
+  </si>
+  <si>
+    <t>POWERMECH</t>
+  </si>
+  <si>
+    <t>INE211R01019</t>
+  </si>
+  <si>
+    <t>PVR LTD</t>
+  </si>
+  <si>
+    <t>PVR</t>
+  </si>
+  <si>
+    <t>INE191H01014</t>
+  </si>
+  <si>
     <t>RailTel Corporation of India L</t>
   </si>
   <si>
@@ -532,9 +611,6 @@
     <t>INE493A01019</t>
   </si>
   <si>
-    <t>30-04-2021</t>
-  </si>
-  <si>
     <t>20-05-2021</t>
   </si>
   <si>
@@ -583,10 +659,13 @@
     <t>INE066O01014</t>
   </si>
   <si>
-    <t>dsfsdfsdf</t>
-  </si>
-  <si>
-    <t>sdfsdfsdf</t>
+    <t>gjhgjh</t>
+  </si>
+  <si>
+    <t>hjkhkj</t>
+  </si>
+  <si>
+    <t>ghjghj</t>
   </si>
 </sst>
 </file>
@@ -989,10 +1068,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U83"/>
+  <dimension ref="A1:U95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
@@ -1038,7 +1117,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>187</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="13" x14ac:dyDescent="0.15">
@@ -1046,7 +1125,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>188</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="13" x14ac:dyDescent="0.15">
@@ -1054,7 +1133,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>188</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="13" x14ac:dyDescent="0.15"/>
@@ -1071,7 +1150,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="10">
-        <v>9150.8799999999992</v>
+        <v>11876.13</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="13" x14ac:dyDescent="0.15">
@@ -1079,7 +1158,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="10">
-        <v>8161.03</v>
+        <v>10671.19</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="13" x14ac:dyDescent="0.15">
@@ -1105,7 +1184,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="10">
-        <v>0.21</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="13" x14ac:dyDescent="0.15">
@@ -1113,7 +1192,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="10">
-        <v>9.82</v>
+        <v>10.96</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="13" x14ac:dyDescent="0.15">
@@ -1121,7 +1200,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="10">
-        <v>8.68</v>
+        <v>11.62</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="13" x14ac:dyDescent="0.15">
@@ -1129,7 +1208,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="10">
-        <v>666</v>
+        <v>721.5</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="13" x14ac:dyDescent="0.15">
@@ -1137,7 +1216,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="10">
-        <v>123.14</v>
+        <v>133.83000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="13" x14ac:dyDescent="0.15">
@@ -1145,7 +1224,7 @@
         <v>15</v>
       </c>
       <c r="B19" s="10">
-        <v>169</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="13" x14ac:dyDescent="0.15">
@@ -1153,7 +1232,7 @@
         <v>16</v>
       </c>
       <c r="B20" s="10">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="13" x14ac:dyDescent="0.15">
@@ -1161,7 +1240,7 @@
         <v>17</v>
       </c>
       <c r="B21" s="10">
-        <v>989.85</v>
+        <v>1086.1600000000001</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="13" x14ac:dyDescent="0.15">
@@ -1811,8 +1890,8 @@
       <c r="A35" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B35" s="11">
-        <v>500085</v>
+      <c r="B35" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>76</v>
@@ -1824,343 +1903,343 @@
         <v>42</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="G35" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H35" s="10">
-        <v>229.55</v>
+        <v>821.95</v>
       </c>
       <c r="I35" s="10">
-        <v>459.1</v>
+        <v>821.95</v>
       </c>
       <c r="J35" s="9" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="K35" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L35" s="10">
-        <v>299.39999999999998</v>
+        <v>1299</v>
       </c>
       <c r="M35" s="10">
-        <v>598.79999999999995</v>
+        <v>1299</v>
       </c>
       <c r="N35" s="11">
-        <v>92</v>
+        <v>158</v>
       </c>
       <c r="O35" s="10">
-        <v>139.69999999999999</v>
+        <v>477.05</v>
       </c>
       <c r="P35" s="10">
-        <v>139.69999999999999</v>
+        <v>477.05</v>
       </c>
       <c r="Q35" s="10"/>
       <c r="R35" s="10"/>
       <c r="S35" s="10"/>
       <c r="T35" s="10"/>
       <c r="U35" s="10">
-        <v>598.79999999999995</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="36" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A36" s="9" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B36" s="11">
-        <v>532848</v>
+        <v>500085</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E36" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="G36" s="11">
         <v>2</v>
       </c>
       <c r="H36" s="10">
-        <v>153.5</v>
+        <v>229.55</v>
       </c>
       <c r="I36" s="10">
-        <v>307</v>
+        <v>459.1</v>
       </c>
       <c r="J36" s="9" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="K36" s="11">
         <v>2</v>
       </c>
       <c r="L36" s="10">
-        <v>183.8</v>
+        <v>299.39999999999998</v>
       </c>
       <c r="M36" s="10">
-        <v>367.6</v>
+        <v>598.79999999999995</v>
       </c>
       <c r="N36" s="11">
-        <v>59</v>
+        <v>92</v>
       </c>
       <c r="O36" s="10">
-        <v>60.6</v>
+        <v>139.69999999999999</v>
       </c>
       <c r="P36" s="10">
-        <v>60.6</v>
+        <v>139.69999999999999</v>
       </c>
       <c r="Q36" s="10"/>
       <c r="R36" s="10"/>
       <c r="S36" s="10"/>
       <c r="T36" s="10"/>
       <c r="U36" s="10">
-        <v>367.6</v>
+        <v>598.79999999999995</v>
       </c>
     </row>
     <row r="37" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A37" s="9" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B37" s="11">
-        <v>532848</v>
+        <v>532783</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E37" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="G37" s="11">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="H37" s="10">
-        <v>153.5</v>
+        <v>74.75</v>
       </c>
       <c r="I37" s="10">
-        <v>460.5</v>
+        <v>1644.5</v>
       </c>
       <c r="J37" s="9" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="K37" s="11">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="L37" s="10">
-        <v>183.8</v>
+        <v>65.8</v>
       </c>
       <c r="M37" s="10">
-        <v>551.4</v>
+        <v>1447.6</v>
       </c>
       <c r="N37" s="11">
-        <v>59</v>
+        <v>91</v>
       </c>
       <c r="O37" s="10">
-        <v>90.9</v>
+        <v>-196.9</v>
       </c>
       <c r="P37" s="10">
-        <v>90.9</v>
+        <v>-196.9</v>
       </c>
       <c r="Q37" s="10"/>
       <c r="R37" s="10"/>
       <c r="S37" s="10"/>
       <c r="T37" s="10"/>
       <c r="U37" s="10">
-        <v>551.4</v>
+        <v>1447.6</v>
       </c>
     </row>
     <row r="38" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A38" s="9" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="B38" s="11">
         <v>532848</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E38" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="G38" s="11">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H38" s="10">
-        <v>145.15</v>
+        <v>153.5</v>
       </c>
       <c r="I38" s="10">
-        <v>725.75</v>
+        <v>307</v>
       </c>
       <c r="J38" s="9" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="K38" s="11">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L38" s="10">
         <v>183.8</v>
       </c>
       <c r="M38" s="10">
-        <v>919</v>
+        <v>367.6</v>
       </c>
       <c r="N38" s="11">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="O38" s="10">
-        <v>193.25</v>
+        <v>60.6</v>
       </c>
       <c r="P38" s="10">
-        <v>193.25</v>
+        <v>60.6</v>
       </c>
       <c r="Q38" s="10"/>
       <c r="R38" s="10"/>
       <c r="S38" s="10"/>
       <c r="T38" s="10"/>
       <c r="U38" s="10">
-        <v>919</v>
+        <v>367.6</v>
       </c>
     </row>
     <row r="39" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A39" s="9" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="B39" s="11">
         <v>532848</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E39" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="G39" s="11">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H39" s="10">
-        <v>147.35</v>
+        <v>153.5</v>
       </c>
       <c r="I39" s="10">
-        <v>736.75</v>
+        <v>460.5</v>
       </c>
       <c r="J39" s="9" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="K39" s="11">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L39" s="10">
         <v>183.8</v>
       </c>
       <c r="M39" s="10">
-        <v>919</v>
+        <v>551.4</v>
       </c>
       <c r="N39" s="11">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="O39" s="10">
-        <v>182.25</v>
+        <v>90.9</v>
       </c>
       <c r="P39" s="10">
-        <v>182.25</v>
+        <v>90.9</v>
       </c>
       <c r="Q39" s="10"/>
       <c r="R39" s="10"/>
       <c r="S39" s="10"/>
       <c r="T39" s="10"/>
       <c r="U39" s="10">
-        <v>919</v>
+        <v>551.4</v>
       </c>
     </row>
     <row r="40" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A40" s="9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B40" s="11">
-        <v>500495</v>
+        <v>532848</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E40" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G40" s="11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H40" s="10">
-        <v>1277</v>
+        <v>145.15</v>
       </c>
       <c r="I40" s="10">
-        <v>5108</v>
+        <v>725.75</v>
       </c>
       <c r="J40" s="9" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K40" s="11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L40" s="10">
-        <v>1271.2</v>
+        <v>183.8</v>
       </c>
       <c r="M40" s="10">
-        <v>5084.8</v>
+        <v>919</v>
       </c>
       <c r="N40" s="11">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="O40" s="10">
-        <v>-23.2</v>
-      </c>
-      <c r="P40" s="10"/>
+        <v>193.25</v>
+      </c>
+      <c r="P40" s="10">
+        <v>193.25</v>
+      </c>
       <c r="Q40" s="10"/>
-      <c r="R40" s="10">
-        <v>-23.2</v>
-      </c>
+      <c r="R40" s="10"/>
       <c r="S40" s="10"/>
       <c r="T40" s="10"/>
       <c r="U40" s="10">
-        <v>23.2</v>
+        <v>919</v>
       </c>
     </row>
     <row r="41" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A41" s="9" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B41" s="11">
-        <v>500940</v>
+        <v>532848</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E41" s="9" t="s">
         <v>42</v>
@@ -2169,1181 +2248,1181 @@
         <v>92</v>
       </c>
       <c r="G41" s="11">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H41" s="10">
-        <v>653</v>
+        <v>147.35</v>
       </c>
       <c r="I41" s="10">
-        <v>5224</v>
+        <v>736.75</v>
       </c>
       <c r="J41" s="9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="K41" s="11">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="L41" s="10">
-        <v>636.79999999999995</v>
+        <v>183.8</v>
       </c>
       <c r="M41" s="10">
-        <v>5094.3999999999996</v>
+        <v>919</v>
       </c>
       <c r="N41" s="11">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="O41" s="10">
-        <v>-129.6</v>
+        <v>182.25</v>
       </c>
       <c r="P41" s="10">
-        <v>-129.6</v>
+        <v>182.25</v>
       </c>
       <c r="Q41" s="10"/>
       <c r="R41" s="10"/>
       <c r="S41" s="10"/>
       <c r="T41" s="10"/>
       <c r="U41" s="10">
-        <v>5094.3999999999996</v>
+        <v>919</v>
       </c>
     </row>
     <row r="42" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A42" s="9" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B42" s="11">
-        <v>500940</v>
+        <v>500495</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E42" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="G42" s="11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H42" s="10">
-        <v>653</v>
+        <v>1277</v>
       </c>
       <c r="I42" s="10">
-        <v>653</v>
+        <v>5108</v>
       </c>
       <c r="J42" s="9" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="K42" s="11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L42" s="10">
-        <v>636.79999999999995</v>
+        <v>1271.2</v>
       </c>
       <c r="M42" s="10">
-        <v>636.79999999999995</v>
+        <v>5084.8</v>
       </c>
       <c r="N42" s="11">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="O42" s="10">
-        <v>-16.2</v>
-      </c>
-      <c r="P42" s="10">
-        <v>-16.2</v>
-      </c>
+        <v>-23.2</v>
+      </c>
+      <c r="P42" s="10"/>
       <c r="Q42" s="10"/>
-      <c r="R42" s="10"/>
+      <c r="R42" s="10">
+        <v>-23.2</v>
+      </c>
       <c r="S42" s="10"/>
       <c r="T42" s="10"/>
       <c r="U42" s="10">
-        <v>636.79999999999995</v>
+        <v>23.2</v>
       </c>
     </row>
     <row r="43" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A43" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B43" s="11">
+        <v>500495</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D43" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="B43" s="11">
-        <v>514167</v>
-      </c>
-      <c r="C43" s="9" t="s">
+      <c r="E43" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F43" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="D43" s="9" t="s">
+      <c r="G43" s="11">
+        <v>1</v>
+      </c>
+      <c r="H43" s="10">
+        <v>1277.05</v>
+      </c>
+      <c r="I43" s="10">
+        <v>1277.05</v>
+      </c>
+      <c r="J43" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="E43" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F43" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="G43" s="11">
-        <v>8</v>
-      </c>
-      <c r="H43" s="10">
-        <v>665.95</v>
-      </c>
-      <c r="I43" s="10">
-        <v>5327.6</v>
-      </c>
-      <c r="J43" s="9" t="s">
-        <v>93</v>
-      </c>
       <c r="K43" s="11">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="L43" s="10">
-        <v>589.35</v>
+        <v>1363.5</v>
       </c>
       <c r="M43" s="10">
-        <v>4714.8</v>
+        <v>1363.5</v>
       </c>
       <c r="N43" s="11">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="O43" s="10">
-        <v>-612.79999999999995</v>
+        <v>86.45</v>
       </c>
       <c r="P43" s="10">
-        <v>-612.79999999999995</v>
+        <v>86.45</v>
       </c>
       <c r="Q43" s="10"/>
       <c r="R43" s="10"/>
       <c r="S43" s="10"/>
       <c r="T43" s="10"/>
       <c r="U43" s="10">
-        <v>4714.8</v>
+        <v>1363.5</v>
       </c>
     </row>
     <row r="44" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A44" s="9" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B44" s="11">
-        <v>532482</v>
+        <v>500495</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E44" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G44" s="11">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="H44" s="10">
-        <v>365.05</v>
+        <v>1277.0999999999999</v>
       </c>
       <c r="I44" s="10">
-        <v>4015.55</v>
+        <v>3831.3</v>
       </c>
       <c r="J44" s="9" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="K44" s="11">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="L44" s="10">
-        <v>303.64999999999998</v>
+        <v>1363.5</v>
       </c>
       <c r="M44" s="10">
-        <v>3340.15</v>
+        <v>4090.5</v>
       </c>
       <c r="N44" s="11">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O44" s="10">
-        <v>-675.4</v>
+        <v>259.2</v>
       </c>
       <c r="P44" s="10">
-        <v>-675.4</v>
+        <v>259.2</v>
       </c>
       <c r="Q44" s="10"/>
       <c r="R44" s="10"/>
       <c r="S44" s="10"/>
       <c r="T44" s="10"/>
       <c r="U44" s="10">
-        <v>3340.15</v>
+        <v>4090.5</v>
       </c>
     </row>
     <row r="45" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A45" s="9" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B45" s="11">
-        <v>532482</v>
+        <v>500495</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="E45" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G45" s="11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H45" s="10">
-        <v>365.05</v>
+        <v>1350.45</v>
       </c>
       <c r="I45" s="10">
-        <v>730.1</v>
+        <v>5401.8</v>
       </c>
       <c r="J45" s="9" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="K45" s="11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L45" s="10">
-        <v>303.8</v>
+        <v>1348.5</v>
       </c>
       <c r="M45" s="10">
-        <v>607.6</v>
+        <v>5394</v>
       </c>
       <c r="N45" s="11">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="O45" s="10">
-        <v>-122.5</v>
-      </c>
-      <c r="P45" s="10">
-        <v>-122.5</v>
-      </c>
+        <v>-7.8</v>
+      </c>
+      <c r="P45" s="10"/>
       <c r="Q45" s="10"/>
-      <c r="R45" s="10"/>
+      <c r="R45" s="10">
+        <v>-7.8</v>
+      </c>
       <c r="S45" s="10"/>
       <c r="T45" s="10"/>
       <c r="U45" s="10">
-        <v>607.6</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="46" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A46" s="9" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B46" s="11">
-        <v>509631</v>
+        <v>526227</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E46" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="G46" s="11">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="H46" s="10">
-        <v>2345.8000000000002</v>
+        <v>99</v>
       </c>
       <c r="I46" s="10">
-        <v>2345.8000000000002</v>
+        <v>1782</v>
       </c>
       <c r="J46" s="9" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="K46" s="11">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="L46" s="10">
-        <v>2363.0500000000002</v>
+        <v>112.75</v>
       </c>
       <c r="M46" s="10">
-        <v>2363.0500000000002</v>
+        <v>2029.5</v>
       </c>
       <c r="N46" s="11">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="O46" s="10">
-        <v>17.25</v>
+        <v>247.5</v>
       </c>
       <c r="P46" s="10">
-        <v>17.25</v>
+        <v>247.5</v>
       </c>
       <c r="Q46" s="10"/>
       <c r="R46" s="10"/>
       <c r="S46" s="10"/>
       <c r="T46" s="10"/>
       <c r="U46" s="10">
-        <v>2363.0500000000002</v>
+        <v>2029.5</v>
       </c>
     </row>
     <row r="47" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A47" s="9" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="B47" s="11">
-        <v>532187</v>
+        <v>526227</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E47" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="G47" s="11">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="H47" s="10">
-        <v>1029.5</v>
+        <v>99</v>
       </c>
       <c r="I47" s="10">
-        <v>1029.5</v>
+        <v>3168</v>
       </c>
       <c r="J47" s="9" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="K47" s="11">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="L47" s="10">
-        <v>1021.35</v>
+        <v>112.75</v>
       </c>
       <c r="M47" s="10">
-        <v>1021.35</v>
+        <v>3608</v>
       </c>
       <c r="N47" s="11">
-        <v>100</v>
+        <v>6</v>
       </c>
       <c r="O47" s="10">
-        <v>-8.15</v>
+        <v>440</v>
       </c>
       <c r="P47" s="10">
-        <v>-8.15</v>
+        <v>440</v>
       </c>
       <c r="Q47" s="10"/>
       <c r="R47" s="10"/>
       <c r="S47" s="10"/>
       <c r="T47" s="10"/>
       <c r="U47" s="10">
-        <v>1021.35</v>
+        <v>3608</v>
       </c>
     </row>
     <row r="48" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A48" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B48" s="11">
+        <v>500940</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="G48" s="11">
+        <v>8</v>
+      </c>
+      <c r="H48" s="10">
+        <v>653</v>
+      </c>
+      <c r="I48" s="10">
+        <v>5224</v>
+      </c>
+      <c r="J48" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="B48" s="11">
-        <v>532187</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="D48" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="E48" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F48" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="G48" s="11">
-        <v>1</v>
-      </c>
-      <c r="H48" s="10">
-        <v>995.2</v>
-      </c>
-      <c r="I48" s="10">
-        <v>995.2</v>
-      </c>
-      <c r="J48" s="9" t="s">
-        <v>113</v>
-      </c>
       <c r="K48" s="11">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="L48" s="10">
-        <v>1021.3</v>
+        <v>636.79999999999995</v>
       </c>
       <c r="M48" s="10">
-        <v>1021.3</v>
+        <v>5094.3999999999996</v>
       </c>
       <c r="N48" s="11">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="O48" s="10">
-        <v>26.1</v>
+        <v>-129.6</v>
       </c>
       <c r="P48" s="10">
-        <v>26.1</v>
+        <v>-129.6</v>
       </c>
       <c r="Q48" s="10"/>
       <c r="R48" s="10"/>
       <c r="S48" s="10"/>
       <c r="T48" s="10"/>
       <c r="U48" s="10">
-        <v>1021.3</v>
+        <v>5094.3999999999996</v>
       </c>
     </row>
     <row r="49" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A49" s="9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B49" s="11">
-        <v>532187</v>
+        <v>500940</v>
       </c>
       <c r="C49" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D49" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="D49" s="9" t="s">
-        <v>111</v>
-      </c>
       <c r="E49" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>73</v>
+        <v>108</v>
       </c>
       <c r="G49" s="11">
         <v>1</v>
       </c>
       <c r="H49" s="10">
-        <v>862.4</v>
+        <v>653</v>
       </c>
       <c r="I49" s="10">
-        <v>862.4</v>
+        <v>653</v>
       </c>
       <c r="J49" s="9" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="K49" s="11">
         <v>1</v>
       </c>
       <c r="L49" s="10">
-        <v>1021.3</v>
+        <v>636.79999999999995</v>
       </c>
       <c r="M49" s="10">
-        <v>1021.3</v>
+        <v>636.79999999999995</v>
       </c>
       <c r="N49" s="11">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="O49" s="10">
-        <v>158.9</v>
+        <v>-16.2</v>
       </c>
       <c r="P49" s="10">
-        <v>158.9</v>
+        <v>-16.2</v>
       </c>
       <c r="Q49" s="10"/>
       <c r="R49" s="10"/>
       <c r="S49" s="10"/>
       <c r="T49" s="10"/>
       <c r="U49" s="10">
-        <v>1021.3</v>
+        <v>636.79999999999995</v>
       </c>
     </row>
     <row r="50" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A50" s="9" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B50" s="11">
-        <v>541179</v>
+        <v>514167</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E50" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F50" s="9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G50" s="11">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="H50" s="10">
-        <v>427.65</v>
+        <v>665.95</v>
       </c>
       <c r="I50" s="10">
-        <v>1282.95</v>
+        <v>5327.6</v>
       </c>
       <c r="J50" s="9" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="K50" s="11">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="L50" s="10">
-        <v>490</v>
+        <v>589.35</v>
       </c>
       <c r="M50" s="10">
-        <v>1470</v>
+        <v>4714.8</v>
       </c>
       <c r="N50" s="11">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="O50" s="10">
-        <v>187.05</v>
+        <v>-612.79999999999995</v>
       </c>
       <c r="P50" s="10">
-        <v>187.05</v>
+        <v>-612.79999999999995</v>
       </c>
       <c r="Q50" s="10"/>
       <c r="R50" s="10"/>
       <c r="S50" s="10"/>
       <c r="T50" s="10"/>
       <c r="U50" s="10">
-        <v>1470</v>
+        <v>4714.8</v>
       </c>
     </row>
     <row r="51" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A51" s="9" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B51" s="11">
-        <v>500219</v>
+        <v>532482</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E51" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F51" s="9" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="G51" s="11">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="H51" s="10">
-        <v>23.15</v>
+        <v>365.05</v>
       </c>
       <c r="I51" s="10">
-        <v>1157.5</v>
+        <v>4015.55</v>
       </c>
       <c r="J51" s="9" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="K51" s="11">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="L51" s="10">
-        <v>31.35</v>
+        <v>303.64999999999998</v>
       </c>
       <c r="M51" s="10">
-        <v>1567.5</v>
+        <v>3340.15</v>
       </c>
       <c r="N51" s="11">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="O51" s="10">
-        <v>410</v>
+        <v>-675.4</v>
       </c>
       <c r="P51" s="10">
-        <v>410</v>
+        <v>-675.4</v>
       </c>
       <c r="Q51" s="10"/>
       <c r="R51" s="10"/>
       <c r="S51" s="10"/>
       <c r="T51" s="10"/>
       <c r="U51" s="10">
-        <v>1567.5</v>
+        <v>3340.15</v>
       </c>
     </row>
     <row r="52" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A52" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B52" s="11">
+        <v>532482</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D52" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="B52" s="11">
-        <v>500219</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="D52" s="9" t="s">
-        <v>123</v>
-      </c>
       <c r="E52" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F52" s="9" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="G52" s="11">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="H52" s="10">
-        <v>23.15</v>
+        <v>365.05</v>
       </c>
       <c r="I52" s="10">
-        <v>1157.5</v>
+        <v>730.1</v>
       </c>
       <c r="J52" s="9" t="s">
-        <v>63</v>
+        <v>109</v>
       </c>
       <c r="K52" s="11">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="L52" s="10">
-        <v>33.35</v>
+        <v>303.8</v>
       </c>
       <c r="M52" s="10">
-        <v>1667.5</v>
+        <v>607.6</v>
       </c>
       <c r="N52" s="11">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="O52" s="10">
-        <v>510</v>
+        <v>-122.5</v>
       </c>
       <c r="P52" s="10">
-        <v>510</v>
+        <v>-122.5</v>
       </c>
       <c r="Q52" s="10"/>
       <c r="R52" s="10"/>
       <c r="S52" s="10"/>
       <c r="T52" s="10"/>
       <c r="U52" s="10">
-        <v>1667.5</v>
+        <v>607.6</v>
       </c>
     </row>
     <row r="53" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A53" s="9" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B53" s="11">
-        <v>590104</v>
+        <v>509631</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E53" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F53" s="9" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G53" s="11">
         <v>1</v>
       </c>
       <c r="H53" s="10">
-        <v>320.39999999999998</v>
+        <v>2345.8000000000002</v>
       </c>
       <c r="I53" s="10">
-        <v>320.39999999999998</v>
+        <v>2345.8000000000002</v>
       </c>
       <c r="J53" s="9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="K53" s="11">
         <v>1</v>
       </c>
       <c r="L53" s="10">
-        <v>404.51</v>
+        <v>2363.0500000000002</v>
       </c>
       <c r="M53" s="10">
-        <v>404.51</v>
+        <v>2363.0500000000002</v>
       </c>
       <c r="N53" s="11">
-        <v>213</v>
+        <v>23</v>
       </c>
       <c r="O53" s="10">
-        <v>84.11</v>
+        <v>17.25</v>
       </c>
       <c r="P53" s="10">
-        <v>84.11</v>
+        <v>17.25</v>
       </c>
       <c r="Q53" s="10"/>
       <c r="R53" s="10"/>
       <c r="S53" s="10"/>
       <c r="T53" s="10"/>
       <c r="U53" s="10">
-        <v>404.51</v>
+        <v>2363.0500000000002</v>
       </c>
     </row>
     <row r="54" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B54" s="11">
-        <v>590104</v>
+        <v>532187</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E54" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F54" s="9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G54" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H54" s="10">
-        <v>324.5</v>
+        <v>1029.5</v>
       </c>
       <c r="I54" s="10">
-        <v>973.5</v>
+        <v>1029.5</v>
       </c>
       <c r="J54" s="9" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="K54" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L54" s="10">
-        <v>404.5</v>
+        <v>1021.35</v>
       </c>
       <c r="M54" s="10">
-        <v>1213.5</v>
+        <v>1021.35</v>
       </c>
       <c r="N54" s="11">
-        <v>193</v>
+        <v>100</v>
       </c>
       <c r="O54" s="10">
-        <v>240</v>
+        <v>-8.15</v>
       </c>
       <c r="P54" s="10">
-        <v>240</v>
+        <v>-8.15</v>
       </c>
       <c r="Q54" s="10"/>
       <c r="R54" s="10"/>
       <c r="S54" s="10"/>
       <c r="T54" s="10"/>
       <c r="U54" s="10">
-        <v>1213.5</v>
+        <v>1021.35</v>
       </c>
     </row>
     <row r="55" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A55" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B55" s="11">
-        <v>590104</v>
+        <v>532187</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E55" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F55" s="9" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="G55" s="11">
         <v>1</v>
       </c>
       <c r="H55" s="10">
-        <v>362.84</v>
+        <v>995.2</v>
       </c>
       <c r="I55" s="10">
-        <v>362.84</v>
+        <v>995.2</v>
       </c>
       <c r="J55" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K55" s="11">
         <v>1</v>
       </c>
       <c r="L55" s="10">
-        <v>360.85</v>
+        <v>1021.3</v>
       </c>
       <c r="M55" s="10">
-        <v>360.85</v>
+        <v>1021.3</v>
       </c>
       <c r="N55" s="11">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="O55" s="10">
-        <v>-1.99</v>
-      </c>
-      <c r="P55" s="10"/>
+        <v>26.1</v>
+      </c>
+      <c r="P55" s="10">
+        <v>26.1</v>
+      </c>
       <c r="Q55" s="10"/>
-      <c r="R55" s="10">
-        <v>-1.99</v>
-      </c>
+      <c r="R55" s="10"/>
       <c r="S55" s="10"/>
       <c r="T55" s="10"/>
       <c r="U55" s="10">
-        <v>1.99</v>
+        <v>1021.3</v>
       </c>
     </row>
     <row r="56" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A56" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B56" s="11">
-        <v>590104</v>
+        <v>532187</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E56" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F56" s="9" t="s">
-        <v>122</v>
+        <v>73</v>
       </c>
       <c r="G56" s="11">
         <v>1</v>
       </c>
       <c r="H56" s="10">
-        <v>404.65</v>
+        <v>862.4</v>
       </c>
       <c r="I56" s="10">
-        <v>404.65</v>
+        <v>862.4</v>
       </c>
       <c r="J56" s="9" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="K56" s="11">
         <v>1</v>
       </c>
       <c r="L56" s="10">
-        <v>404.51</v>
+        <v>1021.3</v>
       </c>
       <c r="M56" s="10">
-        <v>404.51</v>
+        <v>1021.3</v>
       </c>
       <c r="N56" s="11">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="O56" s="10">
-        <v>-0.14000000000000001</v>
-      </c>
-      <c r="P56" s="10"/>
+        <v>158.9</v>
+      </c>
+      <c r="P56" s="10">
+        <v>158.9</v>
+      </c>
       <c r="Q56" s="10"/>
-      <c r="R56" s="10">
-        <v>-0.14000000000000001</v>
-      </c>
+      <c r="R56" s="10"/>
       <c r="S56" s="10"/>
       <c r="T56" s="10"/>
       <c r="U56" s="10">
-        <v>0.14000000000000001</v>
+        <v>1021.3</v>
       </c>
     </row>
     <row r="57" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A57" s="9" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B57" s="11">
-        <v>532714</v>
+        <v>541179</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E57" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F57" s="9" t="s">
-        <v>54</v>
+        <v>133</v>
       </c>
       <c r="G57" s="11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H57" s="10">
-        <v>458.5</v>
+        <v>427.65</v>
       </c>
       <c r="I57" s="10">
-        <v>1834</v>
+        <v>1282.95</v>
       </c>
       <c r="J57" s="9" t="s">
-        <v>55</v>
+        <v>134</v>
       </c>
       <c r="K57" s="11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L57" s="10">
-        <v>418.1</v>
+        <v>490</v>
       </c>
       <c r="M57" s="10">
-        <v>1672.4</v>
+        <v>1470</v>
       </c>
       <c r="N57" s="11">
-        <v>92</v>
+        <v>21</v>
       </c>
       <c r="O57" s="10">
-        <v>-161.6</v>
+        <v>187.05</v>
       </c>
       <c r="P57" s="10">
-        <v>-161.6</v>
+        <v>187.05</v>
       </c>
       <c r="Q57" s="10"/>
       <c r="R57" s="10"/>
       <c r="S57" s="10"/>
       <c r="T57" s="10"/>
       <c r="U57" s="10">
-        <v>1672.4</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="58" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A58" s="9" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B58" s="11">
-        <v>540222</v>
+        <v>500219</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="E58" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F58" s="9" t="s">
-        <v>84</v>
+        <v>124</v>
       </c>
       <c r="G58" s="11">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="H58" s="10">
-        <v>481.2</v>
+        <v>23.15</v>
       </c>
       <c r="I58" s="10">
-        <v>962.4</v>
+        <v>1157.5</v>
       </c>
       <c r="J58" s="9" t="s">
-        <v>113</v>
+        <v>138</v>
       </c>
       <c r="K58" s="11">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="L58" s="10">
-        <v>534.15</v>
+        <v>31.35</v>
       </c>
       <c r="M58" s="10">
-        <v>1068.3</v>
+        <v>1567.5</v>
       </c>
       <c r="N58" s="11">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="O58" s="10">
-        <v>105.9</v>
+        <v>410</v>
       </c>
       <c r="P58" s="10">
-        <v>105.9</v>
+        <v>410</v>
       </c>
       <c r="Q58" s="10"/>
       <c r="R58" s="10"/>
       <c r="S58" s="10"/>
       <c r="T58" s="10"/>
       <c r="U58" s="10">
-        <v>1068.3</v>
+        <v>1567.5</v>
       </c>
     </row>
     <row r="59" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A59" s="9" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B59" s="11">
-        <v>590096</v>
+        <v>500219</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E59" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F59" s="9" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="G59" s="11">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="H59" s="10">
-        <v>1000</v>
+        <v>23.15</v>
       </c>
       <c r="I59" s="10">
-        <v>40000</v>
+        <v>1157.5</v>
       </c>
       <c r="J59" s="9" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="K59" s="11">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="L59" s="10">
-        <v>999.99</v>
+        <v>33.35</v>
       </c>
       <c r="M59" s="10">
-        <v>39999.599999999999</v>
+        <v>1667.5</v>
       </c>
       <c r="N59" s="11">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="O59" s="10">
-        <v>-0.4</v>
+        <v>510</v>
       </c>
       <c r="P59" s="10">
-        <v>-0.4</v>
+        <v>510</v>
       </c>
       <c r="Q59" s="10"/>
       <c r="R59" s="10"/>
       <c r="S59" s="10"/>
       <c r="T59" s="10"/>
       <c r="U59" s="10">
-        <v>39999.599999999999</v>
+        <v>1667.5</v>
       </c>
     </row>
     <row r="60" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A60" s="9" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B60" s="11">
-        <v>523704</v>
+        <v>590104</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D60" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F60" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="G60" s="11">
+        <v>1</v>
+      </c>
+      <c r="H60" s="10">
+        <v>320.39999999999998</v>
+      </c>
+      <c r="I60" s="10">
+        <v>320.39999999999998</v>
+      </c>
+      <c r="J60" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="E60" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F60" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="G60" s="11">
-        <v>2</v>
-      </c>
-      <c r="H60" s="10">
-        <v>1230</v>
-      </c>
-      <c r="I60" s="10">
-        <v>2460</v>
-      </c>
-      <c r="J60" s="9" t="s">
-        <v>139</v>
-      </c>
       <c r="K60" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L60" s="10">
-        <v>2493.1</v>
+        <v>404.51</v>
       </c>
       <c r="M60" s="10">
-        <v>4986.2</v>
+        <v>404.51</v>
       </c>
       <c r="N60" s="11">
-        <v>154</v>
+        <v>213</v>
       </c>
       <c r="O60" s="10">
-        <v>2526.1999999999998</v>
+        <v>84.11</v>
       </c>
       <c r="P60" s="10">
-        <v>2526.1999999999998</v>
+        <v>84.11</v>
       </c>
       <c r="Q60" s="10"/>
       <c r="R60" s="10"/>
       <c r="S60" s="10"/>
       <c r="T60" s="10"/>
       <c r="U60" s="10">
-        <v>4986.2</v>
+        <v>404.51</v>
       </c>
     </row>
     <row r="61" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A61" s="9" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B61" s="11">
-        <v>523704</v>
+        <v>590104</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D61" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F61" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="G61" s="11">
+        <v>3</v>
+      </c>
+      <c r="H61" s="10">
+        <v>324.5</v>
+      </c>
+      <c r="I61" s="10">
+        <v>973.5</v>
+      </c>
+      <c r="J61" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="E61" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F61" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="G61" s="11">
-        <v>2</v>
-      </c>
-      <c r="H61" s="10">
-        <v>1230</v>
-      </c>
-      <c r="I61" s="10">
-        <v>2460</v>
-      </c>
-      <c r="J61" s="9" t="s">
-        <v>139</v>
-      </c>
       <c r="K61" s="11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L61" s="10">
-        <v>2498</v>
+        <v>404.5</v>
       </c>
       <c r="M61" s="10">
-        <v>4996</v>
+        <v>1213.5</v>
       </c>
       <c r="N61" s="11">
-        <v>154</v>
+        <v>193</v>
       </c>
       <c r="O61" s="10">
-        <v>2536</v>
+        <v>240</v>
       </c>
       <c r="P61" s="10">
-        <v>2536</v>
+        <v>240</v>
       </c>
       <c r="Q61" s="10"/>
       <c r="R61" s="10"/>
       <c r="S61" s="10"/>
       <c r="T61" s="10"/>
       <c r="U61" s="10">
-        <v>4996</v>
+        <v>1213.5</v>
       </c>
     </row>
     <row r="62" spans="1:21" ht="13" x14ac:dyDescent="0.15">
@@ -3351,56 +3430,56 @@
         <v>140</v>
       </c>
       <c r="B62" s="11">
-        <v>533286</v>
+        <v>590104</v>
       </c>
       <c r="C62" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="D62" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="D62" s="9" t="s">
-        <v>142</v>
-      </c>
       <c r="E62" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F62" s="9" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G62" s="11">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H62" s="10">
-        <v>167.3</v>
+        <v>362.84</v>
       </c>
       <c r="I62" s="10">
-        <v>836.5</v>
+        <v>362.84</v>
       </c>
       <c r="J62" s="9" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="K62" s="11">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L62" s="10">
-        <v>180.7</v>
+        <v>360.85</v>
       </c>
       <c r="M62" s="10">
-        <v>903.5</v>
+        <v>360.85</v>
       </c>
       <c r="N62" s="11">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="O62" s="10">
-        <v>67</v>
-      </c>
-      <c r="P62" s="10">
-        <v>67</v>
-      </c>
+        <v>-1.99</v>
+      </c>
+      <c r="P62" s="10"/>
       <c r="Q62" s="10"/>
-      <c r="R62" s="10"/>
+      <c r="R62" s="10">
+        <v>-1.99</v>
+      </c>
       <c r="S62" s="10"/>
       <c r="T62" s="10"/>
       <c r="U62" s="10">
-        <v>903.5</v>
+        <v>1.99</v>
       </c>
     </row>
     <row r="63" spans="1:21" ht="13" x14ac:dyDescent="0.15">
@@ -3408,355 +3487,355 @@
         <v>140</v>
       </c>
       <c r="B63" s="11">
-        <v>533286</v>
+        <v>590104</v>
       </c>
       <c r="C63" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="D63" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="D63" s="9" t="s">
-        <v>142</v>
-      </c>
       <c r="E63" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F63" s="9" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="G63" s="11">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H63" s="10">
-        <v>178.25</v>
+        <v>404.65</v>
       </c>
       <c r="I63" s="10">
-        <v>891.25</v>
+        <v>404.65</v>
       </c>
       <c r="J63" s="9" t="s">
-        <v>113</v>
+        <v>138</v>
       </c>
       <c r="K63" s="11">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L63" s="10">
-        <v>180.7</v>
+        <v>404.51</v>
       </c>
       <c r="M63" s="10">
-        <v>903.5</v>
+        <v>404.51</v>
       </c>
       <c r="N63" s="11">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="O63" s="10">
-        <v>12.25</v>
-      </c>
-      <c r="P63" s="10">
-        <v>12.25</v>
-      </c>
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="P63" s="10"/>
       <c r="Q63" s="10"/>
-      <c r="R63" s="10"/>
+      <c r="R63" s="10">
+        <v>-0.14000000000000001</v>
+      </c>
       <c r="S63" s="10"/>
       <c r="T63" s="10"/>
       <c r="U63" s="10">
-        <v>903.5</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="64" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A64" s="9" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B64" s="11">
-        <v>533286</v>
+        <v>532714</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="E64" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F64" s="9" t="s">
-        <v>145</v>
+        <v>54</v>
       </c>
       <c r="G64" s="11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H64" s="10">
-        <v>188.8</v>
+        <v>458.5</v>
       </c>
       <c r="I64" s="10">
-        <v>566.4</v>
+        <v>1834</v>
       </c>
       <c r="J64" s="9" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
       <c r="K64" s="11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L64" s="10">
-        <v>180.7</v>
+        <v>418.1</v>
       </c>
       <c r="M64" s="10">
-        <v>542.1</v>
+        <v>1672.4</v>
       </c>
       <c r="N64" s="11">
-        <v>21</v>
+        <v>92</v>
       </c>
       <c r="O64" s="10">
-        <v>-24.3</v>
+        <v>-161.6</v>
       </c>
       <c r="P64" s="10">
-        <v>-24.3</v>
+        <v>-161.6</v>
       </c>
       <c r="Q64" s="10"/>
       <c r="R64" s="10"/>
       <c r="S64" s="10"/>
       <c r="T64" s="10"/>
       <c r="U64" s="10">
-        <v>542.1</v>
+        <v>1672.4</v>
       </c>
     </row>
     <row r="65" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A65" s="9" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="B65" s="11">
-        <v>533286</v>
+        <v>532942</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="D65" s="9" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="E65" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F65" s="9" t="s">
-        <v>145</v>
+        <v>54</v>
       </c>
       <c r="G65" s="11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H65" s="10">
-        <v>188.8</v>
+        <v>207.3</v>
       </c>
       <c r="I65" s="10">
-        <v>377.6</v>
+        <v>829.2</v>
       </c>
       <c r="J65" s="9" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="K65" s="11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L65" s="10">
-        <v>180.7</v>
+        <v>303.60000000000002</v>
       </c>
       <c r="M65" s="10">
-        <v>361.4</v>
+        <v>1214.4000000000001</v>
       </c>
       <c r="N65" s="11">
-        <v>21</v>
+        <v>183</v>
       </c>
       <c r="O65" s="10">
-        <v>-16.2</v>
+        <v>385.2</v>
       </c>
       <c r="P65" s="10">
-        <v>-16.2</v>
+        <v>385.2</v>
       </c>
       <c r="Q65" s="10"/>
       <c r="R65" s="10"/>
       <c r="S65" s="10"/>
       <c r="T65" s="10"/>
       <c r="U65" s="10">
-        <v>361.4</v>
+        <v>1214.4000000000001</v>
       </c>
     </row>
     <row r="66" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A66" s="9" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B66" s="11">
-        <v>532504</v>
+        <v>532942</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="E66" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F66" s="9" t="s">
-        <v>149</v>
+        <v>54</v>
       </c>
       <c r="G66" s="11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H66" s="10">
-        <v>2573.9</v>
+        <v>207.3</v>
       </c>
       <c r="I66" s="10">
-        <v>2573.9</v>
+        <v>1036.5</v>
       </c>
       <c r="J66" s="9" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="K66" s="11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L66" s="10">
-        <v>3206</v>
+        <v>303.60000000000002</v>
       </c>
       <c r="M66" s="10">
-        <v>3206</v>
+        <v>1518</v>
       </c>
       <c r="N66" s="11">
-        <v>72</v>
+        <v>183</v>
       </c>
       <c r="O66" s="10">
-        <v>632.1</v>
+        <v>481.5</v>
       </c>
       <c r="P66" s="10">
-        <v>632.1</v>
+        <v>481.5</v>
       </c>
       <c r="Q66" s="10"/>
       <c r="R66" s="10"/>
       <c r="S66" s="10"/>
       <c r="T66" s="10"/>
       <c r="U66" s="10">
-        <v>3206</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="67" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A67" s="9" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B67" s="11">
-        <v>539150</v>
+        <v>540222</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E67" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="G67" s="11">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H67" s="10">
-        <v>248.65</v>
+        <v>481.2</v>
       </c>
       <c r="I67" s="10">
-        <v>1491.9</v>
+        <v>962.4</v>
       </c>
       <c r="J67" s="9" t="s">
-        <v>55</v>
+        <v>129</v>
       </c>
       <c r="K67" s="11">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L67" s="10">
-        <v>244.55</v>
+        <v>534.15</v>
       </c>
       <c r="M67" s="10">
-        <v>1467.3</v>
+        <v>1068.3</v>
       </c>
       <c r="N67" s="11">
-        <v>92</v>
+        <v>27</v>
       </c>
       <c r="O67" s="10">
-        <v>-24.6</v>
+        <v>105.9</v>
       </c>
       <c r="P67" s="10">
-        <v>-24.6</v>
+        <v>105.9</v>
       </c>
       <c r="Q67" s="10"/>
       <c r="R67" s="10"/>
       <c r="S67" s="10"/>
       <c r="T67" s="10"/>
       <c r="U67" s="10">
-        <v>1467.3</v>
+        <v>1068.3</v>
       </c>
     </row>
     <row r="68" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A68" s="9" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B68" s="11">
-        <v>539150</v>
+        <v>590096</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E68" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>54</v>
+        <v>123</v>
       </c>
       <c r="G68" s="11">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="H68" s="10">
-        <v>248.65</v>
+        <v>1000</v>
       </c>
       <c r="I68" s="10">
-        <v>497.3</v>
+        <v>40000</v>
       </c>
       <c r="J68" s="9" t="s">
-        <v>55</v>
+        <v>156</v>
       </c>
       <c r="K68" s="11">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="L68" s="10">
-        <v>244.55</v>
+        <v>999.99</v>
       </c>
       <c r="M68" s="10">
-        <v>489.1</v>
+        <v>39999.599999999999</v>
       </c>
       <c r="N68" s="11">
-        <v>92</v>
+        <v>6</v>
       </c>
       <c r="O68" s="10">
-        <v>-8.1999999999999993</v>
+        <v>-0.4</v>
       </c>
       <c r="P68" s="10">
-        <v>-8.1999999999999993</v>
+        <v>-0.4</v>
       </c>
       <c r="Q68" s="10"/>
       <c r="R68" s="10"/>
       <c r="S68" s="10"/>
       <c r="T68" s="10"/>
       <c r="U68" s="10">
-        <v>489.1</v>
+        <v>39999.599999999999</v>
       </c>
     </row>
     <row r="69" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A69" s="9" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B69" s="11">
-        <v>543265</v>
+        <v>523704</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E69" s="9" t="s">
         <v>42</v>
@@ -3765,283 +3844,283 @@
         <v>118</v>
       </c>
       <c r="G69" s="11">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H69" s="10">
-        <v>128</v>
+        <v>1230</v>
       </c>
       <c r="I69" s="10">
-        <v>1280</v>
+        <v>2460</v>
       </c>
       <c r="J69" s="9" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="K69" s="11">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="L69" s="10">
-        <v>156</v>
+        <v>2493.1</v>
       </c>
       <c r="M69" s="10">
-        <v>1560</v>
+        <v>4986.2</v>
       </c>
       <c r="N69" s="11">
-        <v>29</v>
+        <v>154</v>
       </c>
       <c r="O69" s="10">
-        <v>280</v>
+        <v>2526.1999999999998</v>
       </c>
       <c r="P69" s="10">
-        <v>280</v>
+        <v>2526.1999999999998</v>
       </c>
       <c r="Q69" s="10"/>
       <c r="R69" s="10"/>
       <c r="S69" s="10"/>
       <c r="T69" s="10"/>
       <c r="U69" s="10">
-        <v>1560</v>
+        <v>4986.2</v>
       </c>
     </row>
     <row r="70" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A70" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="B70" s="11">
+        <v>523704</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="D70" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="E70" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F70" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="G70" s="11">
+        <v>2</v>
+      </c>
+      <c r="H70" s="10">
+        <v>1230</v>
+      </c>
+      <c r="I70" s="10">
+        <v>2460</v>
+      </c>
+      <c r="J70" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K70" s="11">
+        <v>2</v>
+      </c>
+      <c r="L70" s="10">
+        <v>2498</v>
+      </c>
+      <c r="M70" s="10">
+        <v>4996</v>
+      </c>
+      <c r="N70" s="11">
         <v>154</v>
       </c>
-      <c r="B70" s="11">
-        <v>543265</v>
-      </c>
-      <c r="C70" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="D70" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="E70" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F70" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="G70" s="11">
-        <v>10</v>
-      </c>
-      <c r="H70" s="10">
-        <v>133.9</v>
-      </c>
-      <c r="I70" s="10">
-        <v>1339</v>
-      </c>
-      <c r="J70" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="K70" s="11">
-        <v>10</v>
-      </c>
-      <c r="L70" s="10">
-        <v>157.15</v>
-      </c>
-      <c r="M70" s="10">
-        <v>1571.5</v>
-      </c>
-      <c r="N70" s="11">
-        <v>5</v>
-      </c>
       <c r="O70" s="10">
-        <v>232.5</v>
+        <v>2536</v>
       </c>
       <c r="P70" s="10">
-        <v>232.5</v>
+        <v>2536</v>
       </c>
       <c r="Q70" s="10"/>
       <c r="R70" s="10"/>
       <c r="S70" s="10"/>
       <c r="T70" s="10"/>
       <c r="U70" s="10">
-        <v>1571.5</v>
+        <v>4996</v>
       </c>
     </row>
     <row r="71" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A71" s="9" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B71" s="11">
-        <v>532661</v>
+        <v>533286</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E71" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F71" s="9" t="s">
-        <v>49</v>
+        <v>163</v>
       </c>
       <c r="G71" s="11">
         <v>5</v>
       </c>
       <c r="H71" s="10">
-        <v>398.5</v>
+        <v>167.3</v>
       </c>
       <c r="I71" s="10">
-        <v>1992.5</v>
+        <v>836.5</v>
       </c>
       <c r="J71" s="9" t="s">
-        <v>161</v>
+        <v>129</v>
       </c>
       <c r="K71" s="11">
         <v>5</v>
       </c>
       <c r="L71" s="10">
-        <v>445.35</v>
+        <v>180.7</v>
       </c>
       <c r="M71" s="10">
-        <v>2226.75</v>
+        <v>903.5</v>
       </c>
       <c r="N71" s="11">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="O71" s="10">
-        <v>234.25</v>
+        <v>67</v>
       </c>
       <c r="P71" s="10">
-        <v>234.25</v>
+        <v>67</v>
       </c>
       <c r="Q71" s="10"/>
       <c r="R71" s="10"/>
       <c r="S71" s="10"/>
       <c r="T71" s="10"/>
       <c r="U71" s="10">
-        <v>2226.75</v>
+        <v>903.5</v>
       </c>
     </row>
     <row r="72" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A72" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B72" s="11">
+        <v>533286</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="D72" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="B72" s="11">
-        <v>532915</v>
-      </c>
-      <c r="C72" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="D72" s="9" t="s">
+      <c r="E72" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F72" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="E72" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F72" s="9" t="s">
-        <v>114</v>
-      </c>
       <c r="G72" s="11">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="H72" s="10">
-        <v>97</v>
+        <v>178.25</v>
       </c>
       <c r="I72" s="10">
-        <v>4462</v>
+        <v>891.25</v>
       </c>
       <c r="J72" s="9" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="K72" s="11">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="L72" s="10">
-        <v>87.35</v>
+        <v>180.7</v>
       </c>
       <c r="M72" s="10">
-        <v>4018.1</v>
+        <v>903.5</v>
       </c>
       <c r="N72" s="11">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="O72" s="10">
-        <v>-443.9</v>
+        <v>12.25</v>
       </c>
       <c r="P72" s="10">
-        <v>-443.9</v>
+        <v>12.25</v>
       </c>
       <c r="Q72" s="10"/>
       <c r="R72" s="10"/>
       <c r="S72" s="10"/>
       <c r="T72" s="10"/>
       <c r="U72" s="10">
-        <v>4018.1</v>
+        <v>903.5</v>
       </c>
     </row>
     <row r="73" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A73" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B73" s="11">
+        <v>533286</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="D73" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="B73" s="11">
-        <v>532915</v>
-      </c>
-      <c r="C73" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="D73" s="9" t="s">
-        <v>164</v>
-      </c>
       <c r="E73" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F73" s="9" t="s">
-        <v>114</v>
+        <v>165</v>
       </c>
       <c r="G73" s="11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H73" s="10">
-        <v>97</v>
+        <v>188.8</v>
       </c>
       <c r="I73" s="10">
-        <v>388</v>
+        <v>566.4</v>
       </c>
       <c r="J73" s="9" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="K73" s="11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L73" s="10">
-        <v>87.35</v>
+        <v>180.7</v>
       </c>
       <c r="M73" s="10">
-        <v>349.4</v>
+        <v>542.1</v>
       </c>
       <c r="N73" s="11">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="O73" s="10">
-        <v>-38.6</v>
+        <v>-24.3</v>
       </c>
       <c r="P73" s="10">
-        <v>-38.6</v>
+        <v>-24.3</v>
       </c>
       <c r="Q73" s="10"/>
       <c r="R73" s="10"/>
       <c r="S73" s="10"/>
       <c r="T73" s="10"/>
       <c r="U73" s="10">
-        <v>349.4</v>
+        <v>542.1</v>
       </c>
     </row>
     <row r="74" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A74" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B74" s="11">
+        <v>533286</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="D74" s="9" t="s">
         <v>162</v>
-      </c>
-      <c r="B74" s="11">
-        <v>532915</v>
-      </c>
-      <c r="C74" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="D74" s="9" t="s">
-        <v>164</v>
       </c>
       <c r="E74" s="9" t="s">
         <v>42</v>
@@ -4050,109 +4129,109 @@
         <v>165</v>
       </c>
       <c r="G74" s="11">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H74" s="10">
-        <v>104.6</v>
+        <v>188.8</v>
       </c>
       <c r="I74" s="10">
-        <v>1046</v>
+        <v>377.6</v>
       </c>
       <c r="J74" s="9" t="s">
-        <v>166</v>
+        <v>129</v>
       </c>
       <c r="K74" s="11">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="L74" s="10">
-        <v>117</v>
+        <v>180.7</v>
       </c>
       <c r="M74" s="10">
-        <v>1170</v>
+        <v>361.4</v>
       </c>
       <c r="N74" s="11">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="O74" s="10">
-        <v>124</v>
+        <v>-16.2</v>
       </c>
       <c r="P74" s="10">
-        <v>124</v>
+        <v>-16.2</v>
       </c>
       <c r="Q74" s="10"/>
       <c r="R74" s="10"/>
       <c r="S74" s="10"/>
       <c r="T74" s="10"/>
       <c r="U74" s="10">
-        <v>1170</v>
+        <v>361.4</v>
       </c>
     </row>
     <row r="75" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A75" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B75" s="11">
+        <v>532504</v>
+      </c>
+      <c r="C75" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="B75" s="11">
-        <v>532301</v>
-      </c>
-      <c r="C75" s="9" t="s">
+      <c r="D75" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="D75" s="9" t="s">
+      <c r="E75" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F75" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="E75" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F75" s="9" t="s">
-        <v>170</v>
-      </c>
       <c r="G75" s="11">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H75" s="10">
-        <v>131.94999999999999</v>
+        <v>2573.9</v>
       </c>
       <c r="I75" s="10">
-        <v>1319.5</v>
+        <v>2573.9</v>
       </c>
       <c r="J75" s="9" t="s">
-        <v>171</v>
+        <v>129</v>
       </c>
       <c r="K75" s="11">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="L75" s="10">
-        <v>183.5</v>
+        <v>3206</v>
       </c>
       <c r="M75" s="10">
-        <v>1835</v>
+        <v>3206</v>
       </c>
       <c r="N75" s="11">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="O75" s="10">
-        <v>515.5</v>
+        <v>632.1</v>
       </c>
       <c r="P75" s="10">
-        <v>515.5</v>
+        <v>632.1</v>
       </c>
       <c r="Q75" s="10"/>
       <c r="R75" s="10"/>
       <c r="S75" s="10"/>
       <c r="T75" s="10"/>
       <c r="U75" s="10">
-        <v>1835</v>
+        <v>3206</v>
       </c>
     </row>
     <row r="76" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A76" s="9" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B76" s="11">
-        <v>532301</v>
+        <v>539150</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="D76" s="9" t="s">
         <v>172</v>
@@ -4161,423 +4240,1107 @@
         <v>42</v>
       </c>
       <c r="F76" s="9" t="s">
-        <v>144</v>
+        <v>54</v>
       </c>
       <c r="G76" s="11">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H76" s="10">
-        <v>152</v>
+        <v>248.65</v>
       </c>
       <c r="I76" s="10">
-        <v>760</v>
+        <v>1491.9</v>
       </c>
       <c r="J76" s="9" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="K76" s="11">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L76" s="10">
-        <v>176.75</v>
+        <v>244.55</v>
       </c>
       <c r="M76" s="10">
-        <v>883.75</v>
+        <v>1467.3</v>
       </c>
       <c r="N76" s="11">
-        <v>27</v>
+        <v>92</v>
       </c>
       <c r="O76" s="10">
-        <v>123.75</v>
+        <v>-24.6</v>
       </c>
       <c r="P76" s="10">
-        <v>123.75</v>
+        <v>-24.6</v>
       </c>
       <c r="Q76" s="10"/>
       <c r="R76" s="10"/>
       <c r="S76" s="10"/>
       <c r="T76" s="10"/>
       <c r="U76" s="10">
-        <v>883.75</v>
+        <v>1467.3</v>
       </c>
     </row>
     <row r="77" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A77" s="9" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B77" s="11">
-        <v>532301</v>
+        <v>539150</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="E77" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F77" s="9" t="s">
-        <v>108</v>
+        <v>54</v>
       </c>
       <c r="G77" s="11">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H77" s="10">
-        <v>185.3</v>
+        <v>248.65</v>
       </c>
       <c r="I77" s="10">
-        <v>1853</v>
+        <v>497.3</v>
       </c>
       <c r="J77" s="9" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="K77" s="11">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="L77" s="10">
-        <v>176.75</v>
+        <v>244.55</v>
       </c>
       <c r="M77" s="10">
-        <v>1767.5</v>
+        <v>489.1</v>
       </c>
       <c r="N77" s="11">
-        <v>7</v>
+        <v>92</v>
       </c>
       <c r="O77" s="10">
-        <v>-85.5</v>
+        <v>-8.1999999999999993</v>
       </c>
       <c r="P77" s="10">
-        <v>-85.5</v>
+        <v>-8.1999999999999993</v>
       </c>
       <c r="Q77" s="10"/>
       <c r="R77" s="10"/>
       <c r="S77" s="10"/>
       <c r="T77" s="10"/>
       <c r="U77" s="10">
-        <v>1767.5</v>
+        <v>489.1</v>
       </c>
     </row>
     <row r="78" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A78" s="9" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B78" s="11">
-        <v>500251</v>
+        <v>539302</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E78" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F78" s="9" t="s">
-        <v>93</v>
+        <v>44</v>
       </c>
       <c r="G78" s="11">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H78" s="10">
-        <v>770.6</v>
+        <v>837.6</v>
       </c>
       <c r="I78" s="10">
-        <v>7706</v>
+        <v>837.6</v>
       </c>
       <c r="J78" s="9" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="K78" s="11">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="L78" s="10">
-        <v>765</v>
+        <v>870.85</v>
       </c>
       <c r="M78" s="10">
-        <v>7650</v>
+        <v>870.85</v>
       </c>
       <c r="N78" s="11">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="O78" s="10">
-        <v>-56</v>
-      </c>
-      <c r="P78" s="10"/>
+        <v>33.25</v>
+      </c>
+      <c r="P78" s="10">
+        <v>33.25</v>
+      </c>
       <c r="Q78" s="10"/>
-      <c r="R78" s="10">
-        <v>-56</v>
-      </c>
+      <c r="R78" s="10"/>
       <c r="S78" s="10"/>
       <c r="T78" s="10"/>
       <c r="U78" s="10">
-        <v>56</v>
+        <v>870.85</v>
       </c>
     </row>
     <row r="79" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A79" s="9" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B79" s="11">
-        <v>500251</v>
+        <v>539302</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D79" s="9" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E79" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F79" s="9" t="s">
-        <v>170</v>
+        <v>44</v>
       </c>
       <c r="G79" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H79" s="10">
-        <v>771.55</v>
+        <v>837.55</v>
       </c>
       <c r="I79" s="10">
-        <v>1543.1</v>
+        <v>837.55</v>
       </c>
       <c r="J79" s="9" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="K79" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L79" s="10">
-        <v>852.2</v>
+        <v>870.9</v>
       </c>
       <c r="M79" s="10">
-        <v>1704.4</v>
+        <v>870.9</v>
       </c>
       <c r="N79" s="11">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="O79" s="10">
-        <v>161.30000000000001</v>
+        <v>33.35</v>
       </c>
       <c r="P79" s="10">
-        <v>161.30000000000001</v>
+        <v>33.35</v>
       </c>
       <c r="Q79" s="10"/>
       <c r="R79" s="10"/>
       <c r="S79" s="10"/>
       <c r="T79" s="10"/>
       <c r="U79" s="10">
-        <v>1704.4</v>
+        <v>870.9</v>
       </c>
     </row>
     <row r="80" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A80" s="9" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B80" s="11">
-        <v>500464</v>
+        <v>532689</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E80" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F80" s="9" t="s">
-        <v>179</v>
+        <v>78</v>
       </c>
       <c r="G80" s="11">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H80" s="10">
-        <v>197.55</v>
+        <v>1171.0999999999999</v>
       </c>
       <c r="I80" s="10">
-        <v>1975.5</v>
+        <v>1171.0999999999999</v>
       </c>
       <c r="J80" s="9" t="s">
-        <v>180</v>
+        <v>79</v>
       </c>
       <c r="K80" s="11">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="L80" s="10">
-        <v>170.85</v>
+        <v>1657.55</v>
       </c>
       <c r="M80" s="10">
-        <v>1708.5</v>
+        <v>1657.55</v>
       </c>
       <c r="N80" s="11">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="O80" s="10">
-        <v>-267</v>
+        <v>486.45</v>
       </c>
       <c r="P80" s="10">
-        <v>-267</v>
+        <v>486.45</v>
       </c>
       <c r="Q80" s="10"/>
       <c r="R80" s="10"/>
       <c r="S80" s="10"/>
       <c r="T80" s="10"/>
       <c r="U80" s="10">
-        <v>1708.5</v>
+        <v>1657.55</v>
       </c>
     </row>
     <row r="81" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A81" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="B81" s="11">
+        <v>543265</v>
+      </c>
+      <c r="C81" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="B81" s="11">
-        <v>507685</v>
-      </c>
-      <c r="C81" s="9" t="s">
+      <c r="D81" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="D81" s="9" t="s">
-        <v>183</v>
-      </c>
       <c r="E81" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F81" s="9" t="s">
-        <v>82</v>
+        <v>134</v>
       </c>
       <c r="G81" s="11">
         <v>10</v>
       </c>
       <c r="H81" s="10">
-        <v>554.75</v>
+        <v>128</v>
       </c>
       <c r="I81" s="10">
-        <v>5547.5</v>
+        <v>1280</v>
       </c>
       <c r="J81" s="9" t="s">
-        <v>63</v>
+        <v>183</v>
       </c>
       <c r="K81" s="11">
         <v>10</v>
       </c>
       <c r="L81" s="10">
-        <v>582.35</v>
+        <v>156</v>
       </c>
       <c r="M81" s="10">
-        <v>5823.5</v>
+        <v>1560</v>
       </c>
       <c r="N81" s="11">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="O81" s="10">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="P81" s="10">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="Q81" s="10"/>
       <c r="R81" s="10"/>
       <c r="S81" s="10"/>
       <c r="T81" s="10"/>
       <c r="U81" s="10">
-        <v>5823.5</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="82" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A82" s="9" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B82" s="11">
-        <v>538268</v>
+        <v>543265</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D82" s="9" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E82" s="9" t="s">
         <v>42</v>
       </c>
       <c r="F82" s="9" t="s">
-        <v>170</v>
+        <v>62</v>
       </c>
       <c r="G82" s="11">
+        <v>10</v>
+      </c>
+      <c r="H82" s="10">
+        <v>133.9</v>
+      </c>
+      <c r="I82" s="10">
+        <v>1339</v>
+      </c>
+      <c r="J82" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="K82" s="11">
+        <v>10</v>
+      </c>
+      <c r="L82" s="10">
+        <v>157.15</v>
+      </c>
+      <c r="M82" s="10">
+        <v>1571.5</v>
+      </c>
+      <c r="N82" s="11">
         <v>5</v>
       </c>
-      <c r="H82" s="10">
-        <v>179</v>
-      </c>
-      <c r="I82" s="10">
-        <v>895</v>
-      </c>
-      <c r="J82" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="K82" s="11">
-        <v>5</v>
-      </c>
-      <c r="L82" s="10">
-        <v>251</v>
-      </c>
-      <c r="M82" s="10">
-        <v>1255</v>
-      </c>
-      <c r="N82" s="11">
-        <v>83</v>
-      </c>
       <c r="O82" s="10">
-        <v>360</v>
+        <v>232.5</v>
       </c>
       <c r="P82" s="10">
-        <v>360</v>
+        <v>232.5</v>
       </c>
       <c r="Q82" s="10"/>
       <c r="R82" s="10"/>
       <c r="S82" s="10"/>
       <c r="T82" s="10"/>
       <c r="U82" s="10">
-        <v>1255</v>
+        <v>1571.5</v>
       </c>
     </row>
     <row r="83" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A83" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="B83" s="11">
+        <v>532661</v>
+      </c>
+      <c r="C83" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="D83" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="E83" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F83" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G83" s="11">
+        <v>5</v>
+      </c>
+      <c r="H83" s="10">
+        <v>398.5</v>
+      </c>
+      <c r="I83" s="10">
+        <v>1992.5</v>
+      </c>
+      <c r="J83" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="K83" s="11">
+        <v>5</v>
+      </c>
+      <c r="L83" s="10">
+        <v>445.35</v>
+      </c>
+      <c r="M83" s="10">
+        <v>2226.75</v>
+      </c>
+      <c r="N83" s="11">
+        <v>36</v>
+      </c>
+      <c r="O83" s="10">
+        <v>234.25</v>
+      </c>
+      <c r="P83" s="10">
+        <v>234.25</v>
+      </c>
+      <c r="Q83" s="10"/>
+      <c r="R83" s="10"/>
+      <c r="S83" s="10"/>
+      <c r="T83" s="10"/>
+      <c r="U83" s="10">
+        <v>2226.75</v>
+      </c>
+    </row>
+    <row r="84" spans="1:21" ht="13" x14ac:dyDescent="0.15">
+      <c r="A84" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="B84" s="11">
+        <v>532915</v>
+      </c>
+      <c r="C84" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="D84" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="E84" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F84" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="G84" s="11">
+        <v>46</v>
+      </c>
+      <c r="H84" s="10">
+        <v>97</v>
+      </c>
+      <c r="I84" s="10">
+        <v>4462</v>
+      </c>
+      <c r="J84" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="K84" s="11">
+        <v>46</v>
+      </c>
+      <c r="L84" s="10">
+        <v>87.35</v>
+      </c>
+      <c r="M84" s="10">
+        <v>4018.1</v>
+      </c>
+      <c r="N84" s="11">
+        <v>16</v>
+      </c>
+      <c r="O84" s="10">
+        <v>-443.9</v>
+      </c>
+      <c r="P84" s="10">
+        <v>-443.9</v>
+      </c>
+      <c r="Q84" s="10"/>
+      <c r="R84" s="10"/>
+      <c r="S84" s="10"/>
+      <c r="T84" s="10"/>
+      <c r="U84" s="10">
+        <v>4018.1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:21" ht="13" x14ac:dyDescent="0.15">
+      <c r="A85" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="B85" s="11">
+        <v>532915</v>
+      </c>
+      <c r="C85" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="D85" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="E85" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F85" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="G85" s="11">
+        <v>4</v>
+      </c>
+      <c r="H85" s="10">
+        <v>97</v>
+      </c>
+      <c r="I85" s="10">
+        <v>388</v>
+      </c>
+      <c r="J85" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="K85" s="11">
+        <v>4</v>
+      </c>
+      <c r="L85" s="10">
+        <v>87.35</v>
+      </c>
+      <c r="M85" s="10">
+        <v>349.4</v>
+      </c>
+      <c r="N85" s="11">
+        <v>16</v>
+      </c>
+      <c r="O85" s="10">
+        <v>-38.6</v>
+      </c>
+      <c r="P85" s="10">
+        <v>-38.6</v>
+      </c>
+      <c r="Q85" s="10"/>
+      <c r="R85" s="10"/>
+      <c r="S85" s="10"/>
+      <c r="T85" s="10"/>
+      <c r="U85" s="10">
+        <v>349.4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:21" ht="13" x14ac:dyDescent="0.15">
+      <c r="A86" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="B86" s="11">
+        <v>532915</v>
+      </c>
+      <c r="C86" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="D86" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="E86" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F86" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="G86" s="11">
+        <v>10</v>
+      </c>
+      <c r="H86" s="10">
+        <v>104.6</v>
+      </c>
+      <c r="I86" s="10">
+        <v>1046</v>
+      </c>
+      <c r="J86" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="K86" s="11">
+        <v>10</v>
+      </c>
+      <c r="L86" s="10">
+        <v>117</v>
+      </c>
+      <c r="M86" s="10">
+        <v>1170</v>
+      </c>
+      <c r="N86" s="11">
+        <v>3</v>
+      </c>
+      <c r="O86" s="10">
+        <v>124</v>
+      </c>
+      <c r="P86" s="10">
+        <v>124</v>
+      </c>
+      <c r="Q86" s="10"/>
+      <c r="R86" s="10"/>
+      <c r="S86" s="10"/>
+      <c r="T86" s="10"/>
+      <c r="U86" s="10">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="87" spans="1:21" ht="13" x14ac:dyDescent="0.15">
+      <c r="A87" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="B87" s="11">
+        <v>532301</v>
+      </c>
+      <c r="C87" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="D87" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="E87" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F87" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G87" s="11">
+        <v>10</v>
+      </c>
+      <c r="H87" s="10">
+        <v>131.94999999999999</v>
+      </c>
+      <c r="I87" s="10">
+        <v>1319.5</v>
+      </c>
+      <c r="J87" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="K87" s="11">
+        <v>10</v>
+      </c>
+      <c r="L87" s="10">
+        <v>183.5</v>
+      </c>
+      <c r="M87" s="10">
+        <v>1835</v>
+      </c>
+      <c r="N87" s="11">
+        <v>20</v>
+      </c>
+      <c r="O87" s="10">
+        <v>515.5</v>
+      </c>
+      <c r="P87" s="10">
+        <v>515.5</v>
+      </c>
+      <c r="Q87" s="10"/>
+      <c r="R87" s="10"/>
+      <c r="S87" s="10"/>
+      <c r="T87" s="10"/>
+      <c r="U87" s="10">
+        <v>1835</v>
+      </c>
+    </row>
+    <row r="88" spans="1:21" ht="13" x14ac:dyDescent="0.15">
+      <c r="A88" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="B88" s="11">
+        <v>532301</v>
+      </c>
+      <c r="C88" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="D88" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="E88" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F88" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="G88" s="11">
+        <v>5</v>
+      </c>
+      <c r="H88" s="10">
+        <v>152</v>
+      </c>
+      <c r="I88" s="10">
+        <v>760</v>
+      </c>
+      <c r="J88" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="K88" s="11">
+        <v>5</v>
+      </c>
+      <c r="L88" s="10">
+        <v>176.75</v>
+      </c>
+      <c r="M88" s="10">
+        <v>883.75</v>
+      </c>
+      <c r="N88" s="11">
+        <v>27</v>
+      </c>
+      <c r="O88" s="10">
+        <v>123.75</v>
+      </c>
+      <c r="P88" s="10">
+        <v>123.75</v>
+      </c>
+      <c r="Q88" s="10"/>
+      <c r="R88" s="10"/>
+      <c r="S88" s="10"/>
+      <c r="T88" s="10"/>
+      <c r="U88" s="10">
+        <v>883.75</v>
+      </c>
+    </row>
+    <row r="89" spans="1:21" ht="13" x14ac:dyDescent="0.15">
+      <c r="A89" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="B89" s="11">
+        <v>532301</v>
+      </c>
+      <c r="C89" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="D89" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="E89" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F89" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="G89" s="11">
+        <v>10</v>
+      </c>
+      <c r="H89" s="10">
+        <v>185.3</v>
+      </c>
+      <c r="I89" s="10">
+        <v>1853</v>
+      </c>
+      <c r="J89" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="K89" s="11">
+        <v>10</v>
+      </c>
+      <c r="L89" s="10">
+        <v>176.75</v>
+      </c>
+      <c r="M89" s="10">
+        <v>1767.5</v>
+      </c>
+      <c r="N89" s="11">
+        <v>7</v>
+      </c>
+      <c r="O89" s="10">
+        <v>-85.5</v>
+      </c>
+      <c r="P89" s="10">
+        <v>-85.5</v>
+      </c>
+      <c r="Q89" s="10"/>
+      <c r="R89" s="10"/>
+      <c r="S89" s="10"/>
+      <c r="T89" s="10"/>
+      <c r="U89" s="10">
+        <v>1767.5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:21" ht="13" x14ac:dyDescent="0.15">
+      <c r="A90" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="B90" s="11">
+        <v>500251</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="D90" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="E90" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F90" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="G90" s="11">
+        <v>10</v>
+      </c>
+      <c r="H90" s="10">
+        <v>770.6</v>
+      </c>
+      <c r="I90" s="10">
+        <v>7706</v>
+      </c>
+      <c r="J90" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="K90" s="11">
+        <v>10</v>
+      </c>
+      <c r="L90" s="10">
+        <v>765</v>
+      </c>
+      <c r="M90" s="10">
+        <v>7650</v>
+      </c>
+      <c r="N90" s="11">
+        <v>0</v>
+      </c>
+      <c r="O90" s="10">
+        <v>-56</v>
+      </c>
+      <c r="P90" s="10"/>
+      <c r="Q90" s="10"/>
+      <c r="R90" s="10">
+        <v>-56</v>
+      </c>
+      <c r="S90" s="10"/>
+      <c r="T90" s="10"/>
+      <c r="U90" s="10">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="91" spans="1:21" ht="13" x14ac:dyDescent="0.15">
+      <c r="A91" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="B91" s="11">
+        <v>500251</v>
+      </c>
+      <c r="C91" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="D91" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="E91" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F91" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G91" s="11">
+        <v>2</v>
+      </c>
+      <c r="H91" s="10">
+        <v>771.55</v>
+      </c>
+      <c r="I91" s="10">
+        <v>1543.1</v>
+      </c>
+      <c r="J91" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="K91" s="11">
+        <v>2</v>
+      </c>
+      <c r="L91" s="10">
+        <v>852.2</v>
+      </c>
+      <c r="M91" s="10">
+        <v>1704.4</v>
+      </c>
+      <c r="N91" s="11">
+        <v>33</v>
+      </c>
+      <c r="O91" s="10">
+        <v>161.30000000000001</v>
+      </c>
+      <c r="P91" s="10">
+        <v>161.30000000000001</v>
+      </c>
+      <c r="Q91" s="10"/>
+      <c r="R91" s="10"/>
+      <c r="S91" s="10"/>
+      <c r="T91" s="10"/>
+      <c r="U91" s="10">
+        <v>1704.4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:21" ht="13" x14ac:dyDescent="0.15">
+      <c r="A92" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="B92" s="11">
+        <v>500464</v>
+      </c>
+      <c r="C92" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="D92" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="E92" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F92" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="G92" s="11">
+        <v>10</v>
+      </c>
+      <c r="H92" s="10">
+        <v>197.55</v>
+      </c>
+      <c r="I92" s="10">
+        <v>1975.5</v>
+      </c>
+      <c r="J92" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="K92" s="11">
+        <v>10</v>
+      </c>
+      <c r="L92" s="10">
+        <v>170.85</v>
+      </c>
+      <c r="M92" s="10">
+        <v>1708.5</v>
+      </c>
+      <c r="N92" s="11">
+        <v>7</v>
+      </c>
+      <c r="O92" s="10">
+        <v>-267</v>
+      </c>
+      <c r="P92" s="10">
+        <v>-267</v>
+      </c>
+      <c r="Q92" s="10"/>
+      <c r="R92" s="10"/>
+      <c r="S92" s="10"/>
+      <c r="T92" s="10"/>
+      <c r="U92" s="10">
+        <v>1708.5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:21" ht="13" x14ac:dyDescent="0.15">
+      <c r="A93" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="B93" s="11">
+        <v>507685</v>
+      </c>
+      <c r="C93" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="D93" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="E93" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F93" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G93" s="11">
+        <v>10</v>
+      </c>
+      <c r="H93" s="10">
+        <v>554.75</v>
+      </c>
+      <c r="I93" s="10">
+        <v>5547.5</v>
+      </c>
+      <c r="J93" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="K93" s="11">
+        <v>10</v>
+      </c>
+      <c r="L93" s="10">
+        <v>582.35</v>
+      </c>
+      <c r="M93" s="10">
+        <v>5823.5</v>
+      </c>
+      <c r="N93" s="11">
+        <v>42</v>
+      </c>
+      <c r="O93" s="10">
+        <v>276</v>
+      </c>
+      <c r="P93" s="10">
+        <v>276</v>
+      </c>
+      <c r="Q93" s="10"/>
+      <c r="R93" s="10"/>
+      <c r="S93" s="10"/>
+      <c r="T93" s="10"/>
+      <c r="U93" s="10">
+        <v>5823.5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:21" ht="13" x14ac:dyDescent="0.15">
+      <c r="A94" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="B94" s="11">
+        <v>538268</v>
+      </c>
+      <c r="C94" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="D94" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="E94" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F94" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G94" s="11">
+        <v>5</v>
+      </c>
+      <c r="H94" s="10">
+        <v>179</v>
+      </c>
+      <c r="I94" s="10">
+        <v>895</v>
+      </c>
+      <c r="J94" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="K94" s="11">
+        <v>5</v>
+      </c>
+      <c r="L94" s="10">
+        <v>251</v>
+      </c>
+      <c r="M94" s="10">
+        <v>1255</v>
+      </c>
+      <c r="N94" s="11">
+        <v>83</v>
+      </c>
+      <c r="O94" s="10">
+        <v>360</v>
+      </c>
+      <c r="P94" s="10">
+        <v>360</v>
+      </c>
+      <c r="Q94" s="10"/>
+      <c r="R94" s="10"/>
+      <c r="S94" s="10"/>
+      <c r="T94" s="10"/>
+      <c r="U94" s="10">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="95" spans="1:21" ht="13" x14ac:dyDescent="0.15">
+      <c r="A95" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B83" s="11"/>
-      <c r="C83" s="9"/>
-      <c r="D83" s="9"/>
-      <c r="E83" s="9"/>
-      <c r="F83" s="9"/>
-      <c r="G83" s="11"/>
-      <c r="H83" s="10"/>
-      <c r="I83" s="10"/>
-      <c r="J83" s="9"/>
-      <c r="K83" s="11"/>
-      <c r="L83" s="10"/>
-      <c r="M83" s="10"/>
-      <c r="N83" s="11"/>
-      <c r="O83" s="10">
-        <v>9150.8799999999992</v>
-      </c>
-      <c r="P83" s="10">
-        <v>9232.2099999999991</v>
-      </c>
-      <c r="Q83" s="10">
+      <c r="B95" s="11"/>
+      <c r="C95" s="9"/>
+      <c r="D95" s="9"/>
+      <c r="E95" s="9"/>
+      <c r="F95" s="9"/>
+      <c r="G95" s="11"/>
+      <c r="H95" s="10"/>
+      <c r="I95" s="10"/>
+      <c r="J95" s="9"/>
+      <c r="K95" s="11"/>
+      <c r="L95" s="10"/>
+      <c r="M95" s="10"/>
+      <c r="N95" s="11"/>
+      <c r="O95" s="10">
+        <v>11876.13</v>
+      </c>
+      <c r="P95" s="10">
+        <v>11965.26</v>
+      </c>
+      <c r="Q95" s="10">
         <v>0</v>
       </c>
-      <c r="R83" s="10">
-        <v>-81.33</v>
-      </c>
-      <c r="S83" s="10"/>
-      <c r="T83" s="10">
+      <c r="R95" s="10">
+        <v>-89.13</v>
+      </c>
+      <c r="S95" s="10"/>
+      <c r="T95" s="10">
         <v>0</v>
       </c>
-      <c r="U83" s="10">
-        <v>133340.39000000001</v>
+      <c r="U95" s="10">
+        <v>153317.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>